<commit_message>
:cake: Added the data provider implementation
</commit_message>
<xml_diff>
--- a/src/main/resources/exceldata/Login.xlsx
+++ b/src/main/resources/exceldata/Login.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="LoginDetails" sheetId="2" r:id="rId1"/>
     <sheet name="Details" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="CreateBug" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
   <si>
     <t>UserName</t>
   </si>
@@ -55,6 +55,66 @@
   </si>
   <si>
     <t>Valid</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>blocker</t>
+  </si>
+  <si>
+    <t>critical</t>
+  </si>
+  <si>
+    <t>major</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>minor</t>
+  </si>
+  <si>
+    <t>trivial</t>
+  </si>
+  <si>
+    <t>enhancement</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Macintosh</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>Linux</t>
+  </si>
+  <si>
+    <t>Official music video for Katy Perry's "Roar" brought to you in Junglescope directed by Grady Hall &amp; Mark Kudsi and produced by Javier Jimenez, Danny Lockwood, Patrick Nugent, Derek Johnson and Oualid Mouaness.</t>
+  </si>
+  <si>
+    <t>LMFAO - Party Rock Anthem ft. Lauren Bennett, GoonRock</t>
   </si>
 </sst>
 </file>
@@ -432,11 +492,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -479,9 +542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -554,12 +615,158 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="208.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>